<commit_message>
Estoy ya en la parte de tratamiento post scrapping
</commit_message>
<xml_diff>
--- a/ArchivosDrive/Catalogo_Tripadvisor2.xlsx
+++ b/ArchivosDrive/Catalogo_Tripadvisor2.xlsx
@@ -7761,4 +7761,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c135c4ba-2280-41f8-be7d-6f21d368baa3}" enabled="1" method="Standard" siteId="{24139d14-c62c-4c47-8bdd-ce71ea1d50cf}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>